<commit_message>
Add bitmaps for numbers
</commit_message>
<xml_diff>
--- a/Calculator Keyboard Layout.xlsx
+++ b/Calculator Keyboard Layout.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Microcontroller Development\STM32\Projects\TCalc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83986F2E-5F6D-4C94-BDC0-EFF809BF28FB}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AF1794E-1F30-4E39-B232-E802E0CD2A7A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{D577C607-2841-40D0-89E7-C9680D9FCFA9}"/>
   </bookViews>
@@ -289,9 +289,6 @@
     </r>
   </si>
   <si>
-    <t>Frac</t>
-  </si>
-  <si>
     <t>√</t>
   </si>
   <si>
@@ -396,6 +393,37 @@
   </si>
   <si>
     <t>Cfg</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>b</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -932,8 +960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9AE362B-D102-4015-85AF-9A58578650C2}">
   <dimension ref="A1:AF6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U9" sqref="U9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="36" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1062,7 +1090,7 @@
         <v>18</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L2" s="7" t="s">
         <v>10</v>
@@ -1105,7 +1133,7 @@
         <v>13</v>
       </c>
       <c r="AA2" s="18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AB2" s="12" t="s">
         <v>15</v>
@@ -1150,7 +1178,7 @@
         <v>41</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L3" s="14" t="s">
         <v>42</v>
@@ -1180,22 +1208,22 @@
         <v>41</v>
       </c>
       <c r="U3" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="W3" s="14" t="s">
         <v>42</v>
       </c>
       <c r="X3" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Y3" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Z3" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA3" s="17" t="s">
         <v>55</v>
-      </c>
-      <c r="AA3" s="17" t="s">
-        <v>56</v>
       </c>
       <c r="AB3" s="12" t="s">
         <v>23</v>
@@ -1210,7 +1238,7 @@
         <v>41</v>
       </c>
       <c r="AF3" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:32" ht="36" customHeight="1" x14ac:dyDescent="0.3">
@@ -1263,7 +1291,7 @@
         <v>0</v>
       </c>
       <c r="R4" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="S4" s="12" t="s">
         <v>29</v>
@@ -1325,7 +1353,7 @@
         <v>26</v>
       </c>
       <c r="G5" s="20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>31</v>
@@ -1355,10 +1383,10 @@
         <v>26</v>
       </c>
       <c r="R5" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="S5" s="9" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="T5" s="8" t="s">
         <v>49</v>
@@ -1388,7 +1416,7 @@
         <v>30</v>
       </c>
       <c r="AD5" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AE5" s="11" t="s">
         <v>47</v>
@@ -1414,7 +1442,7 @@
         <v>3</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>27</v>
@@ -1423,10 +1451,10 @@
         <v>33</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L6" s="10" t="s">
         <v>37</v>
@@ -1450,13 +1478,13 @@
         <v>27</v>
       </c>
       <c r="S6" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="T6" s="8" t="s">
         <v>51</v>
       </c>
       <c r="U6" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="W6" s="16" t="s">
         <v>44</v>
@@ -1473,8 +1501,8 @@
       <c r="AA6" s="12">
         <v>3</v>
       </c>
-      <c r="AB6" s="16" t="s">
-        <v>32</v>
+      <c r="AB6" s="19" t="s">
+        <v>65</v>
       </c>
       <c r="AC6" s="16" t="s">
         <v>27</v>
@@ -1483,7 +1511,7 @@
         <v>33</v>
       </c>
       <c r="AE6" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AF6" s="12"/>
     </row>

</xml_diff>

<commit_message>
Change port defs for hardware in 8051
</commit_message>
<xml_diff>
--- a/Calculator Keyboard Layout.xlsx
+++ b/Calculator Keyboard Layout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Microcontroller Development\STM32\Projects\TCalc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AF1794E-1F30-4E39-B232-E802E0CD2A7A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E09B1248-2AA2-4CC7-9F94-D2F3B2CB5D17}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{D577C607-2841-40D0-89E7-C9680D9FCFA9}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="71">
   <si>
     <t>Q</t>
   </si>
@@ -424,6 +424,12 @@
       </rPr>
       <t>b</t>
     </r>
+  </si>
+  <si>
+    <t>Spc</t>
+  </si>
+  <si>
+    <t>Const</t>
   </si>
 </sst>
 </file>
@@ -960,8 +966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9AE362B-D102-4015-85AF-9A58578650C2}">
   <dimension ref="A1:AF6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U9" sqref="U9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="V9" sqref="V9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="36" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1090,7 +1096,7 @@
         <v>18</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="L2" s="7" t="s">
         <v>10</v>
@@ -1119,7 +1125,9 @@
       <c r="T2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="U2" s="12"/>
+      <c r="U2" s="7" t="s">
+        <v>67</v>
+      </c>
       <c r="W2" s="12" t="s">
         <v>10</v>
       </c>
@@ -1513,7 +1521,9 @@
       <c r="AE6" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="AF6" s="12"/>
+      <c r="AF6" s="17" t="s">
+        <v>70</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add 8051 side keyboard code and bitmaps for summation and product
</commit_message>
<xml_diff>
--- a/Calculator Keyboard Layout.xlsx
+++ b/Calculator Keyboard Layout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Microcontroller Development\STM32\Projects\TCalc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E09B1248-2AA2-4CC7-9F94-D2F3B2CB5D17}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B34C450-7184-4D39-AA77-4980E2161778}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{D577C607-2841-40D0-89E7-C9680D9FCFA9}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="75">
   <si>
     <t>Q</t>
   </si>
@@ -121,9 +121,6 @@
   </si>
   <si>
     <t>/</t>
-  </si>
-  <si>
-    <t>EE</t>
   </si>
   <si>
     <t>=</t>
@@ -430,13 +427,28 @@
   </si>
   <si>
     <t>Const</t>
+  </si>
+  <si>
+    <t>Enter</t>
+  </si>
+  <si>
+    <t>[</t>
+  </si>
+  <si>
+    <t>]</t>
+  </si>
+  <si>
+    <t>{</t>
+  </si>
+  <si>
+    <t>}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -539,6 +551,12 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="4">
@@ -588,7 +606,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -648,6 +666,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -967,7 +988,7 @@
   <dimension ref="A1:AF6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="V9" sqref="V9"/>
+      <selection activeCell="W8" sqref="W8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="36" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1096,7 +1117,7 @@
         <v>18</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L2" s="7" t="s">
         <v>10</v>
@@ -1126,7 +1147,7 @@
         <v>18</v>
       </c>
       <c r="U2" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="W2" s="12" t="s">
         <v>10</v>
@@ -1141,7 +1162,7 @@
         <v>13</v>
       </c>
       <c r="AA2" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AB2" s="12" t="s">
         <v>15</v>
@@ -1159,7 +1180,7 @@
     </row>
     <row r="3" spans="1:32" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>19</v>
@@ -1183,13 +1204,13 @@
         <v>25</v>
       </c>
       <c r="I3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="L3" s="14" t="s">
         <v>41</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="L3" s="14" t="s">
-        <v>42</v>
       </c>
       <c r="M3" s="7" t="s">
         <v>19</v>
@@ -1213,25 +1234,25 @@
         <v>25</v>
       </c>
       <c r="T3" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="U3" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="W3" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="U3" s="15" t="s">
+      <c r="X3" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y3" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z3" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="W3" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="X3" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="Y3" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="Z3" s="9" t="s">
+      <c r="AA3" s="17" t="s">
         <v>54</v>
-      </c>
-      <c r="AA3" s="17" t="s">
-        <v>55</v>
       </c>
       <c r="AB3" s="12" t="s">
         <v>23</v>
@@ -1243,18 +1264,18 @@
         <v>25</v>
       </c>
       <c r="AE3" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AF3" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:32" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="C4" s="1">
         <v>7</v>
@@ -1275,16 +1296,16 @@
         <v>29</v>
       </c>
       <c r="I4" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="J4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="L4" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="M4" s="12" t="s">
-        <v>35</v>
+      <c r="L4" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>72</v>
       </c>
       <c r="N4" s="12">
         <v>7</v>
@@ -1299,22 +1320,22 @@
         <v>0</v>
       </c>
       <c r="R4" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="S4" s="12" t="s">
         <v>29</v>
       </c>
       <c r="T4" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="U4" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="W4" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="X4" s="12" t="s">
-        <v>35</v>
+        <v>45</v>
+      </c>
+      <c r="W4" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="X4" s="7" t="s">
+        <v>74</v>
       </c>
       <c r="Y4" s="12">
         <v>7</v>
@@ -1335,18 +1356,18 @@
         <v>29</v>
       </c>
       <c r="AE4" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF4" s="16" t="s">
         <v>38</v>
-      </c>
-      <c r="AF4" s="16" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:32" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C5" s="1">
         <v>4</v>
@@ -1361,22 +1382,22 @@
         <v>26</v>
       </c>
       <c r="G5" s="20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>31</v>
       </c>
       <c r="I5" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="J5" s="2" t="s">
-        <v>48</v>
-      </c>
       <c r="L5" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M5" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N5" s="12">
         <v>4</v>
@@ -1391,22 +1412,22 @@
         <v>26</v>
       </c>
       <c r="R5" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="S5" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="T5" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="U5" s="10" t="s">
         <v>48</v>
       </c>
+      <c r="U5" s="16" t="s">
+        <v>47</v>
+      </c>
       <c r="W5" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="X5" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Y5" s="12">
         <v>4</v>
@@ -1424,21 +1445,21 @@
         <v>30</v>
       </c>
       <c r="AD5" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AE5" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF5" s="16" t="s">
         <v>47</v>
-      </c>
-      <c r="AF5" s="16" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:32" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
@@ -1450,25 +1471,25 @@
         <v>3</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>33</v>
+      <c r="H6" s="21" t="s">
+        <v>70</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L6" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M6" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N6" s="12">
         <v>1</v>
@@ -1479,26 +1500,26 @@
       <c r="P6" s="12">
         <v>3</v>
       </c>
-      <c r="Q6" s="16" t="s">
-        <v>32</v>
+      <c r="Q6" s="19" t="s">
+        <v>64</v>
       </c>
       <c r="R6" s="16" t="s">
         <v>27</v>
       </c>
       <c r="S6" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="T6" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="U6" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="W6" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="X6" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Y6" s="12">
         <v>1</v>
@@ -1510,19 +1531,19 @@
         <v>3</v>
       </c>
       <c r="AB6" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AC6" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="AD6" s="12" t="s">
-        <v>33</v>
+      <c r="AD6" s="7" t="s">
+        <v>32</v>
       </c>
       <c r="AE6" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AF6" s="17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change key mappings for the mixed number and improper fraction keys
</commit_message>
<xml_diff>
--- a/Calculator Keyboard Layout.xlsx
+++ b/Calculator Keyboard Layout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Microcontroller Development\STM32\Projects\TCalc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B34C450-7184-4D39-AA77-4980E2161778}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{97A29EA0-9C36-42D6-8095-9CD463D5917B}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{D577C607-2841-40D0-89E7-C9680D9FCFA9}"/>
   </bookViews>
@@ -313,9 +313,51 @@
     <t>≈</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">a </t>
-    </r>
+    <t>π</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>Graphing</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>×</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>x</t>
+    </r>
+  </si>
+  <si>
+    <t>×</t>
+  </si>
+  <si>
+    <t>Cfg</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <vertAlign val="superscript"/>
@@ -324,7 +366,7 @@
         <rFont val="Consolas"/>
         <family val="3"/>
       </rPr>
-      <t>b</t>
+      <t>a</t>
     </r>
     <r>
       <rPr>
@@ -343,112 +385,106 @@
         <rFont val="Consolas"/>
         <family val="3"/>
       </rPr>
+      <t>b</t>
+    </r>
+  </si>
+  <si>
+    <t>Spc</t>
+  </si>
+  <si>
+    <t>Const</t>
+  </si>
+  <si>
+    <t>Enter</t>
+  </si>
+  <si>
+    <t>[</t>
+  </si>
+  <si>
+    <t>]</t>
+  </si>
+  <si>
+    <t>{</t>
+  </si>
+  <si>
+    <t>}</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>b</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">
+a </t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>b</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
       <t>c</t>
     </r>
-  </si>
-  <si>
-    <t>π</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>Graphing</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>×</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color theme="1"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>10</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>x</t>
-    </r>
-  </si>
-  <si>
-    <t>×</t>
-  </si>
-  <si>
-    <t>Cfg</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>a</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>/</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>b</t>
-    </r>
-  </si>
-  <si>
-    <t>Spc</t>
-  </si>
-  <si>
-    <t>Const</t>
-  </si>
-  <si>
-    <t>Enter</t>
-  </si>
-  <si>
-    <t>[</t>
-  </si>
-  <si>
-    <t>]</t>
-  </si>
-  <si>
-    <t>{</t>
-  </si>
-  <si>
-    <t>}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -554,6 +590,20 @@
     </font>
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Consolas"/>
       <family val="3"/>
@@ -606,7 +656,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -670,6 +720,9 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -987,8 +1040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9AE362B-D102-4015-85AF-9A58578650C2}">
   <dimension ref="A1:AF6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="W8" sqref="W8"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="AC4" sqref="AC4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="36" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1117,7 +1170,7 @@
         <v>18</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L2" s="7" t="s">
         <v>10</v>
@@ -1147,7 +1200,7 @@
         <v>18</v>
       </c>
       <c r="U2" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="W2" s="12" t="s">
         <v>10</v>
@@ -1162,7 +1215,7 @@
         <v>13</v>
       </c>
       <c r="AA2" s="18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AB2" s="12" t="s">
         <v>15</v>
@@ -1302,10 +1355,10 @@
         <v>38</v>
       </c>
       <c r="L4" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="M4" s="7" t="s">
         <v>71</v>
-      </c>
-      <c r="M4" s="7" t="s">
-        <v>72</v>
       </c>
       <c r="N4" s="12">
         <v>7</v>
@@ -1332,10 +1385,10 @@
         <v>45</v>
       </c>
       <c r="W4" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="X4" s="7" t="s">
         <v>73</v>
-      </c>
-      <c r="X4" s="7" t="s">
-        <v>74</v>
       </c>
       <c r="Y4" s="12">
         <v>7</v>
@@ -1382,7 +1435,7 @@
         <v>26</v>
       </c>
       <c r="G5" s="20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>31</v>
@@ -1415,7 +1468,7 @@
         <v>57</v>
       </c>
       <c r="S5" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="T5" s="8" t="s">
         <v>48</v>
@@ -1444,8 +1497,8 @@
       <c r="AC5" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="AD5" s="9" t="s">
-        <v>60</v>
+      <c r="AD5" s="22" t="s">
+        <v>74</v>
       </c>
       <c r="AE5" s="11" t="s">
         <v>46</v>
@@ -1471,19 +1524,19 @@
         <v>3</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>27</v>
       </c>
       <c r="H6" s="21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>51</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L6" s="10" t="s">
         <v>36</v>
@@ -1501,7 +1554,7 @@
         <v>3</v>
       </c>
       <c r="Q6" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="R6" s="16" t="s">
         <v>27</v>
@@ -1513,7 +1566,7 @@
         <v>50</v>
       </c>
       <c r="U6" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="W6" s="16" t="s">
         <v>43</v>
@@ -1531,7 +1584,7 @@
         <v>3</v>
       </c>
       <c r="AB6" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AC6" s="16" t="s">
         <v>27</v>
@@ -1543,7 +1596,7 @@
         <v>51</v>
       </c>
       <c r="AF6" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add constant selection menu
</commit_message>
<xml_diff>
--- a/Calculator Keyboard Layout.xlsx
+++ b/Calculator Keyboard Layout.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Microcontroller Development\STM32\Projects\TCalc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{97A29EA0-9C36-42D6-8095-9CD463D5917B}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA92FFA3-9BB2-46D8-A2A0-69392AD763A5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{D577C607-2841-40D0-89E7-C9680D9FCFA9}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="76">
   <si>
     <t>Q</t>
   </si>
@@ -478,13 +478,17 @@
       </rPr>
       <t>c</t>
     </r>
+  </si>
+  <si>
+    <t>CLR
+VAR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -607,6 +611,13 @@
       <color theme="1"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -656,7 +667,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -722,6 +733,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1040,8 +1054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9AE362B-D102-4015-85AF-9A58578650C2}">
   <dimension ref="A1:AF6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="AC4" sqref="AC4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="36" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1408,8 +1422,8 @@
       <c r="AD4" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="AE4" s="11" t="s">
-        <v>37</v>
+      <c r="AE4" s="23" t="s">
+        <v>75</v>
       </c>
       <c r="AF4" s="16" t="s">
         <v>38</v>

</xml_diff>

<commit_message>
Fix various bugs and add keybind for approx equals key
</commit_message>
<xml_diff>
--- a/Calculator Keyboard Layout.xlsx
+++ b/Calculator Keyboard Layout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Microcontroller Development\STM32\Projects\TCalc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA92FFA3-9BB2-46D8-A2A0-69392AD763A5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{879F1BA4-658E-4C39-AAC7-B45D2E1719F0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{D577C607-2841-40D0-89E7-C9680D9FCFA9}"/>
   </bookViews>
@@ -735,7 +735,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1054,8 +1054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9AE362B-D102-4015-85AF-9A58578650C2}">
   <dimension ref="A1:AF6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U10" sqref="U10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="36" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Add matrix entry handlers
</commit_message>
<xml_diff>
--- a/Calculator Keyboard Layout.xlsx
+++ b/Calculator Keyboard Layout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Microcontroller Development\STM32\Projects\TCalc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{879F1BA4-658E-4C39-AAC7-B45D2E1719F0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D18DD1E-460D-44AD-B7BE-94B2A1598D91}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{D577C607-2841-40D0-89E7-C9680D9FCFA9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D577C607-2841-40D0-89E7-C9680D9FCFA9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="94">
   <si>
     <t>Q</t>
   </si>
@@ -142,9 +142,6 @@
   </si>
   <si>
     <t>AC</t>
-  </si>
-  <si>
-    <t>Cat</t>
   </si>
   <si>
     <t>,</t>
@@ -292,18 +289,6 @@
     <t>Ctrl</t>
   </si>
   <si>
-    <t>Copy</t>
-  </si>
-  <si>
-    <t>Paste</t>
-  </si>
-  <si>
-    <t>Cut</t>
-  </si>
-  <si>
-    <t>Undo</t>
-  </si>
-  <si>
     <t>Π</t>
   </si>
   <si>
@@ -317,9 +302,6 @@
   </si>
   <si>
     <t>e</t>
-  </si>
-  <si>
-    <t>Graphing</t>
   </si>
   <si>
     <r>
@@ -398,18 +380,6 @@
     <t>Enter</t>
   </si>
   <si>
-    <t>[</t>
-  </si>
-  <si>
-    <t>]</t>
-  </si>
-  <si>
-    <t>{</t>
-  </si>
-  <si>
-    <t>}</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <vertAlign val="superscript"/>
@@ -482,13 +452,98 @@
   <si>
     <t>CLR
 VAR</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>FUNC</t>
+  </si>
+  <si>
+    <t>FUNC
+RCLL</t>
+  </si>
+  <si>
+    <t>MAT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -564,12 +619,6 @@
     <font>
       <vertAlign val="superscript"/>
       <sz val="14"/>
-      <color theme="1"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <color theme="1"/>
       <name val="Consolas"/>
       <family val="3"/>
@@ -720,22 +769,22 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1054,8 +1103,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9AE362B-D102-4015-85AF-9A58578650C2}">
   <dimension ref="A1:AF6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U10" sqref="U10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="W9" sqref="W9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="36" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1065,34 +1114,34 @@
   <sheetData>
     <row r="1" spans="1:32" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>67</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>56</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>68</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>69</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>70</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>71</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>7</v>
+        <v>72</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>8</v>
+        <v>73</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>9</v>
+        <v>74</v>
       </c>
       <c r="L1" s="7" t="s">
         <v>0</v>
@@ -1124,67 +1173,67 @@
       <c r="U1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="W1" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="X1" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y1" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z1" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="AA1" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="AB1" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="AC1" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="AD1" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="AE1" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="AF1" s="12" t="s">
-        <v>9</v>
+      <c r="W1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:32" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>75</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>76</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>77</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>13</v>
+        <v>78</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>14</v>
+        <v>79</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>15</v>
+        <v>80</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>16</v>
+        <v>81</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>17</v>
+        <v>82</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>67</v>
+        <v>83</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>59</v>
       </c>
       <c r="L2" s="7" t="s">
         <v>10</v>
@@ -1214,70 +1263,72 @@
         <v>18</v>
       </c>
       <c r="U2" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="W2" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="X2" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y2" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z2" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA2" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="AB2" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="AC2" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="AD2" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="AE2" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="AF2" s="12"/>
+        <v>61</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AF2" s="12" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="3" spans="1:32" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>19</v>
+        <v>84</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>20</v>
+        <v>85</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>21</v>
+        <v>86</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>22</v>
+        <v>87</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>23</v>
+        <v>88</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>24</v>
+        <v>89</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>25</v>
+        <v>90</v>
       </c>
       <c r="I3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="L3" s="14" t="s">
         <v>40</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="L3" s="14" t="s">
-        <v>41</v>
       </c>
       <c r="M3" s="7" t="s">
         <v>19</v>
@@ -1301,40 +1352,40 @@
         <v>25</v>
       </c>
       <c r="T3" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="U3" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="W3" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="U3" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="W3" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="X3" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="Y3" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="Z3" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="AA3" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="AB3" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="AC3" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="AD3" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="AE3" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="AF3" s="15" t="s">
-        <v>52</v>
+      <c r="X3" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AD3" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF3" s="6" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:32" ht="36" customHeight="1" x14ac:dyDescent="0.3">
@@ -1368,11 +1419,11 @@
       <c r="J4" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="L4" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="M4" s="7" t="s">
-        <v>71</v>
+      <c r="L4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="N4" s="12">
         <v>7</v>
@@ -1387,22 +1438,22 @@
         <v>0</v>
       </c>
       <c r="R4" s="7" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="S4" s="12" t="s">
         <v>29</v>
       </c>
       <c r="T4" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="U4" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="W4" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="X4" s="7" t="s">
-        <v>73</v>
+        <v>44</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="Y4" s="12">
         <v>7</v>
@@ -1422,8 +1473,8 @@
       <c r="AD4" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="AE4" s="23" t="s">
-        <v>75</v>
+      <c r="AE4" s="22" t="s">
+        <v>65</v>
       </c>
       <c r="AF4" s="16" t="s">
         <v>38</v>
@@ -1433,8 +1484,8 @@
       <c r="A5" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>39</v>
+      <c r="B5" s="3" t="s">
+        <v>91</v>
       </c>
       <c r="C5" s="1">
         <v>4</v>
@@ -1448,23 +1499,23 @@
       <c r="F5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="20" t="s">
-        <v>64</v>
+      <c r="G5" s="19" t="s">
+        <v>58</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>31</v>
       </c>
       <c r="I5" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>47</v>
       </c>
       <c r="L5" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="M5" s="16" t="s">
-        <v>39</v>
+      <c r="M5" s="23" t="s">
+        <v>92</v>
       </c>
       <c r="N5" s="12">
         <v>4</v>
@@ -1479,22 +1530,22 @@
         <v>26</v>
       </c>
       <c r="R5" s="7" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="S5" s="9" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="T5" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="U5" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="W5" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="X5" s="16" t="s">
-        <v>39</v>
+      <c r="X5" s="13" t="s">
+        <v>91</v>
       </c>
       <c r="Y5" s="12">
         <v>4</v>
@@ -1511,22 +1562,22 @@
       <c r="AC5" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="AD5" s="22" t="s">
-        <v>74</v>
+      <c r="AD5" s="21" t="s">
+        <v>64</v>
       </c>
       <c r="AE5" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF5" s="16" t="s">
         <v>46</v>
-      </c>
-      <c r="AF5" s="16" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:32" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
@@ -1537,26 +1588,26 @@
       <c r="E6" s="1">
         <v>3</v>
       </c>
-      <c r="F6" s="19" t="s">
-        <v>63</v>
+      <c r="F6" s="18" t="s">
+        <v>57</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="21" t="s">
-        <v>69</v>
+      <c r="H6" s="20" t="s">
+        <v>63</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="L6" s="10" t="s">
         <v>36</v>
       </c>
       <c r="M6" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N6" s="12">
         <v>1</v>
@@ -1567,26 +1618,26 @@
       <c r="P6" s="12">
         <v>3</v>
       </c>
-      <c r="Q6" s="19" t="s">
-        <v>63</v>
+      <c r="Q6" s="18" t="s">
+        <v>57</v>
       </c>
       <c r="R6" s="16" t="s">
         <v>27</v>
       </c>
       <c r="S6" s="7" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="T6" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="U6" s="7" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="W6" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="X6" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Y6" s="12">
         <v>1</v>
@@ -1597,8 +1648,8 @@
       <c r="AA6" s="12">
         <v>3</v>
       </c>
-      <c r="AB6" s="19" t="s">
-        <v>63</v>
+      <c r="AB6" s="18" t="s">
+        <v>57</v>
       </c>
       <c r="AC6" s="16" t="s">
         <v>27</v>
@@ -1607,10 +1658,10 @@
         <v>32</v>
       </c>
       <c r="AE6" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AF6" s="17" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change key mappings on keyboard
Move graph function selection to Ctrl+F and make Ctrl+G graph.
</commit_message>
<xml_diff>
--- a/Calculator Keyboard Layout.xlsx
+++ b/Calculator Keyboard Layout.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Microcontroller Development\STM32\Projects\TCalc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D18DD1E-460D-44AD-B7BE-94B2A1598D91}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06AD8C61-1C37-4C21-8155-547ABCA69AC5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D577C607-2841-40D0-89E7-C9680D9FCFA9}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="98">
   <si>
     <t>Q</t>
   </si>
@@ -115,9 +115,6 @@
   </si>
   <si>
     <t>-</t>
-  </si>
-  <si>
-    <t>*</t>
   </si>
   <si>
     <t>/</t>
@@ -205,9 +202,6 @@
       </rPr>
       <t>n</t>
     </r>
-  </si>
-  <si>
-    <t>OFF</t>
   </si>
   <si>
     <r>
@@ -537,13 +531,55 @@
   </si>
   <si>
     <t>MAT</t>
+  </si>
+  <si>
+    <r>
+      <t>{</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="24"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="24"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>b</t>
+    </r>
+  </si>
+  <si>
+    <t>Graph</t>
+  </si>
+  <si>
+    <t>Graph
+Funcs</t>
+  </si>
+  <si>
+    <t>Graph
+Options</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>·</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -636,12 +672,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="18"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Consolas"/>
@@ -667,6 +697,38 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="36"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -689,7 +751,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -712,11 +774,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -775,17 +846,32 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1101,10 +1187,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9AE362B-D102-4015-85AF-9A58578650C2}">
-  <dimension ref="A1:AF6"/>
+  <dimension ref="A1:AF7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="W9" sqref="W9"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="36" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1114,34 +1200,34 @@
   <sheetData>
     <row r="1" spans="1:32" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="L1" s="7" t="s">
         <v>0</v>
@@ -1174,66 +1260,66 @@
         <v>9</v>
       </c>
       <c r="W1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="Y1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AD1" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>74</v>
+      <c r="AF1" s="23" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:32" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="J2" s="12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="L2" s="7" t="s">
         <v>10</v>
@@ -1263,72 +1349,72 @@
         <v>18</v>
       </c>
       <c r="U2" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="W2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="X2" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="Y2" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="Z2" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AA2" s="1" t="s">
+      <c r="Z2" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="AA2" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="AB2" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="AC2" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AD2" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AC2" s="1" t="s">
+      <c r="AE2" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="AD2" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="AE2" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="AF2" s="12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:32" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>90</v>
-      </c>
       <c r="I3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="L3" s="14" t="s">
         <v>39</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="L3" s="14" t="s">
-        <v>40</v>
       </c>
       <c r="M3" s="7" t="s">
         <v>19</v>
@@ -1352,48 +1438,48 @@
         <v>25</v>
       </c>
       <c r="T3" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="U3" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="W3" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="U3" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="W3" s="5" t="s">
-        <v>40</v>
-      </c>
       <c r="X3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Z3" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="Y3" s="1" t="s">
+      <c r="AA3" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="Z3" s="1" t="s">
+      <c r="AB3" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="AA3" s="1" t="s">
+      <c r="AC3" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="AB3" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="AC3" s="1" t="s">
-        <v>89</v>
-      </c>
       <c r="AD3" s="7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="AE3" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AF3" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:32" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="C4" s="1">
         <v>7</v>
@@ -1414,16 +1500,16 @@
         <v>29</v>
       </c>
       <c r="I4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="J4" s="2" t="s">
-        <v>38</v>
-      </c>
       <c r="L4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="N4" s="12">
         <v>7</v>
@@ -1438,22 +1524,22 @@
         <v>0</v>
       </c>
       <c r="R4" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="S4" s="12" t="s">
         <v>29</v>
       </c>
       <c r="T4" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="U4" s="10" t="s">
-        <v>44</v>
+        <v>46</v>
+      </c>
+      <c r="U4" s="16" t="s">
+        <v>37</v>
       </c>
       <c r="W4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="X4" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="X4" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="Y4" s="12">
         <v>7</v>
@@ -1473,19 +1559,19 @@
       <c r="AD4" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="AE4" s="22" t="s">
-        <v>65</v>
+      <c r="AE4" s="21" t="s">
+        <v>63</v>
       </c>
       <c r="AF4" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:32" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C5" s="1">
         <v>4</v>
@@ -1499,23 +1585,23 @@
       <c r="F5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="19" t="s">
-        <v>58</v>
+      <c r="G5" s="28" t="s">
+        <v>97</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="L5" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="M5" s="23" t="s">
-        <v>92</v>
+        <v>34</v>
+      </c>
+      <c r="M5" s="22" t="s">
+        <v>90</v>
       </c>
       <c r="N5" s="12">
         <v>4</v>
@@ -1530,22 +1616,22 @@
         <v>26</v>
       </c>
       <c r="R5" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="S5" s="9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="T5" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="U5" s="16" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="W5" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="X5" s="13" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="Y5" s="12">
         <v>4</v>
@@ -1559,25 +1645,25 @@
       <c r="AB5" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="AC5" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="AD5" s="21" t="s">
-        <v>64</v>
+      <c r="AC5" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD5" s="20" t="s">
+        <v>62</v>
       </c>
       <c r="AE5" s="11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="AF5" s="16" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:32" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
@@ -1589,25 +1675,25 @@
         <v>3</v>
       </c>
       <c r="F6" s="18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="20" t="s">
-        <v>63</v>
+      <c r="H6" s="19" t="s">
+        <v>61</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L6" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M6" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N6" s="12">
         <v>1</v>
@@ -1619,25 +1705,25 @@
         <v>3</v>
       </c>
       <c r="Q6" s="18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="R6" s="16" t="s">
         <v>27</v>
       </c>
       <c r="S6" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T6" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="U6" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="T6" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="U6" s="7" t="s">
-        <v>56</v>
-      </c>
       <c r="W6" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="X6" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Y6" s="12">
         <v>1</v>
@@ -1649,22 +1735,65 @@
         <v>3</v>
       </c>
       <c r="AB6" s="18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="AC6" s="16" t="s">
         <v>27</v>
       </c>
       <c r="AD6" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AE6" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="AF6" s="17" t="s">
-        <v>62</v>
-      </c>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="26"/>
+      <c r="L7" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="M7" s="26"/>
+      <c r="N7" s="26"/>
+      <c r="O7" s="26"/>
+      <c r="P7" s="26"/>
+      <c r="Q7" s="26"/>
+      <c r="R7" s="26"/>
+      <c r="S7" s="26"/>
+      <c r="T7" s="26"/>
+      <c r="U7" s="26"/>
+      <c r="W7" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="X7" s="26"/>
+      <c r="Y7" s="26"/>
+      <c r="Z7" s="26"/>
+      <c r="AA7" s="26"/>
+      <c r="AB7" s="26"/>
+      <c r="AC7" s="26"/>
+      <c r="AD7" s="26"/>
+      <c r="AE7" s="26"/>
+      <c r="AF7" s="26"/>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A7:J7"/>
+    <mergeCell ref="L7:U7"/>
+    <mergeCell ref="W7:AF7"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Add new characters to LCD charset
Add new logic operators to LCD charset, including AND, OR, XOR and NOT.
</commit_message>
<xml_diff>
--- a/Calculator Keyboard Layout.xlsx
+++ b/Calculator Keyboard Layout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Microcontroller Development\STM32\Projects\TCalc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06AD8C61-1C37-4C21-8155-547ABCA69AC5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{436E87A6-BDE5-4AC9-8B3E-9074483DC83E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D577C607-2841-40D0-89E7-C9680D9FCFA9}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="103">
   <si>
     <t>Q</t>
   </si>
@@ -573,6 +573,21 @@
   </si>
   <si>
     <t>·</t>
+  </si>
+  <si>
+    <t>&lt;</t>
+  </si>
+  <si>
+    <t>&gt;</t>
+  </si>
+  <si>
+    <t>≤</t>
+  </si>
+  <si>
+    <t>≥</t>
+  </si>
+  <si>
+    <t>Logic</t>
   </si>
 </sst>
 </file>
@@ -864,13 +879,13 @@
     <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1189,8 +1204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9AE362B-D102-4015-85AF-9A58578650C2}">
   <dimension ref="A1:AF7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="36" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1505,11 +1520,11 @@
       <c r="J4" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="L4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>33</v>
+      <c r="L4" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="M4" s="23" t="s">
+        <v>99</v>
       </c>
       <c r="N4" s="12">
         <v>7</v>
@@ -1535,11 +1550,11 @@
       <c r="U4" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="W4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="X4" s="1" t="s">
-        <v>33</v>
+      <c r="W4" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="X4" s="23" t="s">
+        <v>101</v>
       </c>
       <c r="Y4" s="12">
         <v>7</v>
@@ -1585,7 +1600,7 @@
       <c r="F5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="28" t="s">
+      <c r="G5" s="26" t="s">
         <v>97</v>
       </c>
       <c r="H5" s="1" t="s">
@@ -1597,8 +1612,8 @@
       <c r="J5" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="L5" s="13" t="s">
-        <v>34</v>
+      <c r="L5" s="24" t="s">
+        <v>102</v>
       </c>
       <c r="M5" s="22" t="s">
         <v>90</v>
@@ -1754,39 +1769,39 @@
       <c r="A7" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="26"/>
-      <c r="J7" s="26"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
       <c r="L7" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="M7" s="26"/>
-      <c r="N7" s="26"/>
-      <c r="O7" s="26"/>
-      <c r="P7" s="26"/>
-      <c r="Q7" s="26"/>
-      <c r="R7" s="26"/>
-      <c r="S7" s="26"/>
-      <c r="T7" s="26"/>
-      <c r="U7" s="26"/>
+      <c r="M7" s="28"/>
+      <c r="N7" s="28"/>
+      <c r="O7" s="28"/>
+      <c r="P7" s="28"/>
+      <c r="Q7" s="28"/>
+      <c r="R7" s="28"/>
+      <c r="S7" s="28"/>
+      <c r="T7" s="28"/>
+      <c r="U7" s="28"/>
       <c r="W7" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="X7" s="26"/>
-      <c r="Y7" s="26"/>
-      <c r="Z7" s="26"/>
-      <c r="AA7" s="26"/>
-      <c r="AB7" s="26"/>
-      <c r="AC7" s="26"/>
-      <c r="AD7" s="26"/>
-      <c r="AE7" s="26"/>
-      <c r="AF7" s="26"/>
+      <c r="X7" s="28"/>
+      <c r="Y7" s="28"/>
+      <c r="Z7" s="28"/>
+      <c r="AA7" s="28"/>
+      <c r="AB7" s="28"/>
+      <c r="AC7" s="28"/>
+      <c r="AD7" s="28"/>
+      <c r="AE7" s="28"/>
+      <c r="AF7" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Add right arrow character
Add right arrow character, bound to Shift+-.
</commit_message>
<xml_diff>
--- a/Calculator Keyboard Layout.xlsx
+++ b/Calculator Keyboard Layout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Microcontroller Development\STM32\Projects\TCalc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5E9658F-F7E5-4761-BAEF-1DA58FE303F9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{798686BF-1C77-48ED-8CB9-8073BC5DE3C5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D577C607-2841-40D0-89E7-C9680D9FCFA9}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="105">
   <si>
     <t>Q</t>
   </si>
@@ -591,6 +591,9 @@
   </si>
   <si>
     <t>!</t>
+  </si>
+  <si>
+    <t>→</t>
   </si>
 </sst>
 </file>
@@ -1207,8 +1210,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9AE362B-D102-4015-85AF-9A58578650C2}">
   <dimension ref="A1:AF7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X10" sqref="X10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="V9" sqref="V9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="36" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1544,8 +1547,8 @@
       <c r="R4" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="S4" s="12" t="s">
-        <v>29</v>
+      <c r="S4" s="7" t="s">
+        <v>104</v>
       </c>
       <c r="T4" s="8" t="s">
         <v>46</v>

</xml_diff>

<commit_message>
Add key for subscript
Bind Shift+Exponent to insert a subscript.
</commit_message>
<xml_diff>
--- a/Calculator Keyboard Layout.xlsx
+++ b/Calculator Keyboard Layout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Microcontroller Development\STM32\Projects\TCalc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5E9658F-F7E5-4761-BAEF-1DA58FE303F9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F27174F-D15D-41D0-9C3B-E324C6ED311F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D577C607-2841-40D0-89E7-C9680D9FCFA9}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="105">
   <si>
     <t>Q</t>
   </si>
@@ -591,13 +591,28 @@
   </si>
   <si>
     <t>!</t>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>a</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -747,6 +762,13 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1208,7 +1230,7 @@
   <dimension ref="A1:AF7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X10" sqref="X10"/>
+      <selection activeCell="V8" sqref="V8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="36" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1642,8 +1664,8 @@
       <c r="T5" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="U5" s="16" t="s">
-        <v>44</v>
+      <c r="U5" s="10" t="s">
+        <v>104</v>
       </c>
       <c r="W5" s="13" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
Add processing for absolute value
Add processing for absolute value in eval::evaluate(). Increase version
to 1.2.8 and update keyboard layout.
</commit_message>
<xml_diff>
--- a/Calculator Keyboard Layout.xlsx
+++ b/Calculator Keyboard Layout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Microcontroller Development\STM32\Projects\TCalc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F27174F-D15D-41D0-9C3B-E324C6ED311F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41192192-2F64-489C-A5FF-12ACC983B7E6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D577C607-2841-40D0-89E7-C9680D9FCFA9}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="102">
   <si>
     <t>Q</t>
   </si>
@@ -575,18 +575,6 @@
     <t>·</t>
   </si>
   <si>
-    <t>&lt;</t>
-  </si>
-  <si>
-    <t>&gt;</t>
-  </si>
-  <si>
-    <t>≤</t>
-  </si>
-  <si>
-    <t>≥</t>
-  </si>
-  <si>
     <t>Logic</t>
   </si>
   <si>
@@ -606,6 +594,9 @@
       </rPr>
       <t>a</t>
     </r>
+  </si>
+  <si>
+    <t>|x|</t>
   </si>
 </sst>
 </file>
@@ -1230,7 +1221,7 @@
   <dimension ref="A1:AF7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V8" sqref="V8"/>
+      <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="36" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1478,7 +1469,7 @@
         <v>25</v>
       </c>
       <c r="T3" s="7" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="U3" s="15" t="s">
         <v>49</v>
@@ -1545,11 +1536,11 @@
       <c r="J4" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="L4" s="23" t="s">
-        <v>98</v>
-      </c>
-      <c r="M4" s="23" t="s">
-        <v>99</v>
+      <c r="L4" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="N4" s="12">
         <v>7</v>
@@ -1575,11 +1566,11 @@
       <c r="U4" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="W4" s="23" t="s">
-        <v>100</v>
-      </c>
-      <c r="X4" s="23" t="s">
-        <v>101</v>
+      <c r="W4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="Y4" s="12">
         <v>7</v>
@@ -1638,7 +1629,7 @@
         <v>44</v>
       </c>
       <c r="L5" s="24" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="M5" s="22" t="s">
         <v>90</v>
@@ -1665,7 +1656,7 @@
         <v>45</v>
       </c>
       <c r="U5" s="10" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="W5" s="13" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
Implement the fraction-format key
Implement the fraction-format key to convert result display method from
improper fractions to mixed numbers.
</commit_message>
<xml_diff>
--- a/Calculator Keyboard Layout.xlsx
+++ b/Calculator Keyboard Layout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Microcontroller Development\STM32\Projects\TCalc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBBC573F-C6C1-42CA-9D9B-F4E941A3CDE0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA6203CD-D6A3-440F-B387-9E2B3F44FC89}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D577C607-2841-40D0-89E7-C9680D9FCFA9}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="98">
   <si>
     <t>Q</t>
   </si>
@@ -133,9 +133,6 @@
   </si>
   <si>
     <t>ln</t>
-  </si>
-  <si>
-    <t>DEL</t>
   </si>
   <si>
     <t>AC</t>
@@ -254,32 +251,6 @@
     <t>CLR</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>n</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>√</t>
-    </r>
-  </si>
-  <si>
-    <t>√</t>
-  </si>
-  <si>
     <t>Ctrl</t>
   </si>
   <si>
@@ -331,9 +302,6 @@
     <t>×</t>
   </si>
   <si>
-    <t>Cfg</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <vertAlign val="superscript"/>
@@ -523,47 +491,8 @@
     <t>m</t>
   </si>
   <si>
-    <t>FUNC</t>
-  </si>
-  <si>
     <t>FUNC
 RCLL</t>
-  </si>
-  <si>
-    <r>
-      <t>{</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="24"/>
-        <color theme="1"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>a</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="24"/>
-        <color theme="1"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>b</t>
-    </r>
-  </si>
-  <si>
-    <t>Graph</t>
-  </si>
-  <si>
-    <t>Graph
-Funcs</t>
-  </si>
-  <si>
-    <t>Graph
-Options</t>
   </si>
   <si>
     <t>Normal</t>
@@ -602,20 +531,52 @@
     <t>μ</t>
   </si>
   <si>
-    <t>[x]</t>
-  </si>
-  <si>
     <t>*</t>
   </si>
   <si>
-    <t>|</t>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>A</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>|</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>B</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">
+</t>
+  </si>
+  <si>
+    <t>←</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -747,20 +708,6 @@
       <family val="3"/>
     </font>
     <font>
-      <vertAlign val="superscript"/>
-      <sz val="24"/>
-      <color theme="1"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <vertAlign val="subscript"/>
-      <sz val="24"/>
-      <color theme="1"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
-    <font>
       <sz val="36"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -773,8 +720,15 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <i/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -790,12 +744,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -836,7 +784,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -913,11 +861,8 @@
     <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -940,6 +885,711 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>64858</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>405711</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>401904</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{03DF2433-B1F3-4DC5-9BC9-FAE1C780C3EF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13323658" y="990600"/>
+          <a:ext cx="340853" cy="325704"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>29394</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>121921</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>422812</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>381001</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC5B94E7-8BD4-485B-816F-2892F7AACA07}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14202594" y="121921"/>
+          <a:ext cx="393418" cy="259080"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>53341</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>53341</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>426720</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>426720</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{27C58A21-74D3-4084-9364-DD68A861E3C8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4168141" y="510541"/>
+          <a:ext cx="373379" cy="373379"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>53341</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>53341</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>426720</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>426720</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8E1863B-87E8-49EA-A2D0-5B8FA907D9DC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14226541" y="510541"/>
+          <a:ext cx="373379" cy="373379"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>60960</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>426720</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A84F94E-79BB-40A7-83B2-9894F9F9E8C6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11948160" y="525780"/>
+          <a:ext cx="358140" cy="358140"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>60960</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>350520</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F279BD2D-5304-4A9E-9385-A62C6FBF657E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12405360" y="525780"/>
+          <a:ext cx="281940" cy="281940"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>274321</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>259081</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>449580</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6911CF0C-B515-40FA-9C47-C08120B3DB71}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12618721" y="716281"/>
+          <a:ext cx="190499" cy="190499"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>60960</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09A6F94E-617E-4719-BD01-CA6B53E0DB7A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11490960" y="518160"/>
+          <a:ext cx="281940" cy="281940"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>245166</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>259080</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>449580</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E8C2F23-3F58-442D-8905-3EB8879DBC18}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11675166" y="716280"/>
+          <a:ext cx="212034" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>69905</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>375234</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>388620</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{001FFE4D-1801-4E09-96C2-F804A58EC548}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10585505" y="1943100"/>
+          <a:ext cx="305329" cy="274320"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>77525</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>382854</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>396240</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E8ADA13-3EBA-44BE-B2DA-C0B7C3AB30C1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="534725" y="1950720"/>
+          <a:ext cx="305329" cy="274320"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>60960</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>394293</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>363823</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="24" name="Picture 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14F20C82-0D2F-46F9-BE87-00E9BDE14DE8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8747760" y="2392680"/>
+          <a:ext cx="333333" cy="257143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>45720</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>379053</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>386683</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="26" name="Picture 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66A14C33-D1DC-426A-B580-ABCE3A5345B6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3703320" y="2415540"/>
+          <a:ext cx="333333" cy="257143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>60960</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>394293</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>371443</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="27" name="Picture 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86307AC0-6A6B-4A7C-BAED-1948317D7232}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13776960" y="2400300"/>
+          <a:ext cx="333333" cy="257143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1242,7 +1892,7 @@
   <dimension ref="A1:AF7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="Y10" sqref="Y10"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="36" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1252,34 +1902,34 @@
   <sheetData>
     <row r="1" spans="1:32" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="L1" s="7" t="s">
         <v>0</v>
@@ -1312,67 +1962,63 @@
         <v>9</v>
       </c>
       <c r="W1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="X1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AC1" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="AD1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="AB1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="AC1" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AF1" s="23" t="s">
-        <v>91</v>
-      </c>
+      <c r="AF1" s="23"/>
     </row>
     <row r="2" spans="1:32" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>57</v>
-      </c>
+      <c r="J2" s="12"/>
       <c r="L2" s="7" t="s">
         <v>10</v>
       </c>
@@ -1401,72 +2047,68 @@
         <v>18</v>
       </c>
       <c r="U2" s="7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="Y2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z2" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="AA2" s="24"/>
+      <c r="AB2" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="AC2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="Z2" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="AA2" s="24" t="s">
-        <v>92</v>
-      </c>
-      <c r="AB2" s="25" t="s">
-        <v>94</v>
-      </c>
-      <c r="AC2" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="AD2" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="AE2" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="AF2" s="12" t="s">
-        <v>57</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="AF2" s="12"/>
     </row>
     <row r="3" spans="1:32" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>88</v>
-      </c>
       <c r="I3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="L3" s="14" t="s">
         <v>38</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="L3" s="14" t="s">
-        <v>39</v>
       </c>
       <c r="M3" s="7" t="s">
         <v>19</v>
@@ -1490,40 +2132,38 @@
         <v>25</v>
       </c>
       <c r="T3" s="7" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="U3" s="15" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="W3" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="X3" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AB3" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="Y3" s="1" t="s">
+      <c r="AC3" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="Z3" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="AA3" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="AB3" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="AC3" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="AD3" s="7" t="s">
-        <v>103</v>
-      </c>
+      <c r="AD3" s="7"/>
       <c r="AE3" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AF3" s="6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:32" ht="36" customHeight="1" x14ac:dyDescent="0.3">
@@ -1552,13 +2192,13 @@
         <v>29</v>
       </c>
       <c r="I4" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="J4" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="L4" s="7" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>33</v>
@@ -1567,7 +2207,7 @@
         <v>7</v>
       </c>
       <c r="O4" s="7" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="P4" s="12">
         <v>9</v>
@@ -1576,16 +2216,16 @@
         <v>0</v>
       </c>
       <c r="R4" s="7" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="S4" s="23" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="T4" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="U4" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="W4" s="1" t="s">
         <v>32</v>
@@ -1605,26 +2245,24 @@
       <c r="AB4" s="12">
         <v>0</v>
       </c>
-      <c r="AC4" s="7" t="s">
-        <v>105</v>
+      <c r="AC4" s="9" t="s">
+        <v>95</v>
       </c>
       <c r="AD4" s="12" t="s">
         <v>29</v>
       </c>
       <c r="AE4" s="21" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="AF4" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:32" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>89</v>
-      </c>
+      <c r="B5" s="3"/>
       <c r="C5" s="1">
         <v>4</v>
       </c>
@@ -1638,22 +2276,22 @@
         <v>26</v>
       </c>
       <c r="G5" s="26" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>30</v>
       </c>
       <c r="I5" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="J5" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="L5" s="24" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="M5" s="22" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="N5" s="12">
         <v>4</v>
@@ -1668,23 +2306,21 @@
         <v>26</v>
       </c>
       <c r="R5" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="S5" s="9" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="T5" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="U5" s="10" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="W5" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="X5" s="13" t="s">
-        <v>89</v>
-      </c>
+      <c r="X5" s="13"/>
       <c r="Y5" s="12">
         <v>4</v>
       </c>
@@ -1698,24 +2334,24 @@
         <v>26</v>
       </c>
       <c r="AC5" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="AD5" s="27" t="s">
-        <v>62</v>
+        <v>53</v>
+      </c>
+      <c r="AD5" s="20" t="s">
+        <v>58</v>
       </c>
       <c r="AE5" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF5" s="16" t="s">
         <v>43</v>
-      </c>
-      <c r="AF5" s="16" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:32" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
@@ -1727,25 +2363,23 @@
         <v>3</v>
       </c>
       <c r="F6" s="18" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>27</v>
       </c>
       <c r="H6" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>48</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="I6" s="4"/>
       <c r="J6" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="L6" s="10" t="s">
         <v>35</v>
       </c>
       <c r="M6" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N6" s="12">
         <v>1</v>
@@ -1757,25 +2391,23 @@
         <v>3</v>
       </c>
       <c r="Q6" s="18" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="R6" s="16" t="s">
         <v>27</v>
       </c>
       <c r="S6" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="T6" s="8" t="s">
-        <v>47</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="T6" s="8"/>
       <c r="U6" s="7" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="W6" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="X6" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Y6" s="12">
         <v>1</v>
@@ -1787,7 +2419,7 @@
         <v>3</v>
       </c>
       <c r="AB6" s="18" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="AC6" s="16" t="s">
         <v>27</v>
@@ -1795,50 +2427,48 @@
       <c r="AD6" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="AE6" s="11" t="s">
-        <v>48</v>
-      </c>
+      <c r="AE6" s="11"/>
       <c r="AF6" s="17" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:32" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="28" t="s">
-        <v>95</v>
-      </c>
-      <c r="B7" s="29"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="29"/>
-      <c r="H7" s="29"/>
-      <c r="I7" s="29"/>
-      <c r="J7" s="29"/>
-      <c r="L7" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="M7" s="29"/>
-      <c r="N7" s="29"/>
-      <c r="O7" s="29"/>
-      <c r="P7" s="29"/>
-      <c r="Q7" s="29"/>
-      <c r="R7" s="29"/>
-      <c r="S7" s="29"/>
-      <c r="T7" s="29"/>
-      <c r="U7" s="29"/>
-      <c r="W7" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="X7" s="29"/>
-      <c r="Y7" s="29"/>
-      <c r="Z7" s="29"/>
-      <c r="AA7" s="29"/>
-      <c r="AB7" s="29"/>
-      <c r="AC7" s="29"/>
-      <c r="AD7" s="29"/>
-      <c r="AE7" s="29"/>
-      <c r="AF7" s="29"/>
+      <c r="A7" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" s="28"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
+      <c r="L7" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="M7" s="28"/>
+      <c r="N7" s="28"/>
+      <c r="O7" s="28"/>
+      <c r="P7" s="28"/>
+      <c r="Q7" s="28"/>
+      <c r="R7" s="28"/>
+      <c r="S7" s="28"/>
+      <c r="T7" s="28"/>
+      <c r="U7" s="28"/>
+      <c r="W7" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="X7" s="28"/>
+      <c r="Y7" s="28"/>
+      <c r="Z7" s="28"/>
+      <c r="AA7" s="28"/>
+      <c r="AB7" s="28"/>
+      <c r="AC7" s="28"/>
+      <c r="AD7" s="28"/>
+      <c r="AE7" s="28"/>
+      <c r="AF7" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1848,5 +2478,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>